<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@70e82f59f2c8e5cdd47a125fa85e6a147201451d 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-ncpi-sample.xlsx
+++ b/StructureDefinition-ncpi-sample.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-27T14:40:47+00:00</t>
+    <t>2025-07-21T16:00:02+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -260,7 +260,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}collection-no-parent:If there is no parent sample, collection information must be present. If there is collection information present, there should be no parent sample. {parent.empty() implies collection.exists() and collection.exists() implies parent.empty()}parent-no-collection:If there is no collection information, a parent sample must be present. If there is a parent sample present, there should be no collection information. {collection.empty() implies parent.exists() and parent.exists() implies collection.empty()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}collection-xor-parent:If there is a parent sample, there should be no collection information. If there is collection information present, there should be no parent sample. {parent.exists().not() or collection.exists().not()}</t>
   </si>
   <si>
     <t>Role[classCode=SPEC]</t>
@@ -4628,7 +4628,7 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>84</v>

</xml_diff>